<commit_message>
new updated lines both files
</commit_message>
<xml_diff>
--- a/User.xlsx
+++ b/User.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Git Learning</t>
+  </si>
+  <si>
+    <t>Add line 1</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -373,6 +376,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>